<commit_message>
many teams rotation input complete
</commit_message>
<xml_diff>
--- a/ToDoList_Form.xlsx
+++ b/ToDoList_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Add" sheetId="1" state="visible" r:id="rId1"/>
@@ -1368,8 +1368,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
@@ -1822,7 +1822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2620,42 +2620,42 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05-00-00</t>
+          <t>06-00-00</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>팀빌딩 워크숍</t>
+          <t>경영층 특강 참석자 선정</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>기획팀</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>김문석</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>검토</t>
+          <t>진행</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>22-11-23</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>팀장 지시</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2665,12 +2665,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06-00-00</t>
+          <t>07-00-00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>경영층 특강 참석자 선정</t>
+          <t>센터 주간이슈 논의회</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2710,12 +2710,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>07-00-00</t>
+          <t>07-01-00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>센터 주간이슈 논의회</t>
+          <t>메일 송부</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2749,18 +2749,18 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>08-00-00</t>
+          <t>07-01-01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>경영층 보고</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2794,18 +2794,18 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>09-00-00</t>
+          <t>08-00-00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>회의록 작성</t>
+          <t>경영층 보고</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2840,6 +2840,411 @@
       </c>
       <c r="I24" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>08-01-00</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>완료</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>차체설계1팀</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>08-02-00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>차체설계2팀</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>08-03-00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>차체설계3팀</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>08-04-00</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>외장설계1팀</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>08-05-00</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>dkkkkkkkkkkkkkkkkk</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>08-06-00</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>daaleiw12222222222222222222222</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>08-07-00</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>aksdakalskdfasf</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>08-08-00</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1212123124k</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>08-09-00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>외장설계2팀</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>진행</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still working but not fixing yet
</commit_message>
<xml_diff>
--- a/ToDoList_Form.xlsx
+++ b/ToDoList_Form.xlsx
@@ -1366,13 +1366,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1385,282 +1385,104 @@
           <t>이름</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>분류No</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>전실</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>차체실</t>
         </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>전실</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>클로저실</t>
         </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>전실</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>선행실</t>
         </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>전실</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>외장실</t>
         </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>전팀</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>차체설계1팀</t>
-        </is>
+          <t>내장실</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>전팀</t>
+          <t>바디 전실</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>차체설계2팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>차체설계3팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>외장설계1팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>dkkkkkkkkkkkkkkkkk</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>daaleiw12222222222222222222222</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>aksdakalskdfasf</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1212123124k</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>전팀</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>외장설계2팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>내장실</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>내장설계1팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>내장실</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>내장설계2팀</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>123123alsdkjfalsdkfjddddddddddddddddddd</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>DSDDDDDDDDDDDDDDD</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>1231</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>AAAAAAAAAAAAAAAAAA</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>dskskeie</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>BBBBBBBBBBBBBBBB</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>wiwoiwe</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>CCCC</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>lv,픝</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1123123</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>이이느으</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>DDAAW</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>크크크크ㅡ</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>DDDQ1</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>크크크크ㅡ</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>GTHYYH</t>
-        </is>
+          <t>안전실</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1670,13 +1492,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1689,6 +1511,11 @@
           <t>이름</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>분류No</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1701,6 +1528,9 @@
           <t>차차차</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1710,8 +1540,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>외외외</t>
-        </is>
+          <t>외장책임</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1722,8 +1555,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>클클클</t>
-        </is>
+          <t>내장책임</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1737,6 +1573,9 @@
           <t>홍길동</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1749,17 +1588,23 @@
           <t>박현대</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>팀코디</t>
+          <t>원가</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>최기아</t>
-        </is>
+          <t>가가가</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -1770,8 +1615,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>가가가</t>
-        </is>
+          <t>나나나</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1782,8 +1630,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>나나나</t>
-        </is>
+          <t>다다다</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1794,25 +1645,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>다다다</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>원가</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
           <t>라라라</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2535,17 +2376,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>교육 예산 관리</t>
+          <t>실별 핵심인재 추천</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>전실</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>실코디</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2555,12 +2396,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>22-11-23</t>
+          <t>22-11-26</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12시</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2575,22 +2416,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04-00-00</t>
+          <t>03-01-00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>실별 핵심인재 추천</t>
+          <t>실 추천</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>전실</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>실코디</t>
+          <t>차차차</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2600,12 +2441,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>22-11-26</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12시</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2614,18 +2455,18 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>04-01-00</t>
+          <t>03-01-01</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>실 추천</t>
+          <t>팀장 추천중</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2635,7 +2476,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>차차차</t>
+          <t>홍길동</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2645,17 +2486,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>10/22</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>10시</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>추천서 작성중</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2665,7 +2506,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>04-01-01</t>
+          <t>03-01-02</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2680,7 +2521,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>홍길동</t>
+          <t>박현대</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2710,7 +2551,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04-01-02</t>
+          <t>03-01-03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2725,7 +2566,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>박현대</t>
+          <t>최기아</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2755,12 +2596,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04-01-03</t>
+          <t>03-02-00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>팀장 추천중</t>
+          <t>실 추천</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2770,7 +2611,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>최기아</t>
+          <t>외외외</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2780,17 +2621,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>10/22</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10시</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>추천서 작성중</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2800,22 +2641,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>04-02-00</t>
+          <t>03-02-01</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>실 추천</t>
+          <t>검토중</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>차체설계1팀</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>외외외</t>
+          <t>팀 코디</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2825,17 +2666,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>11라ㅏ아</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>리이니</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>ㄹㅇ라</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2845,7 +2686,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>04-02-01</t>
+          <t>03-02-02</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2855,7 +2696,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>차체설계1팀</t>
+          <t>차체설계2팀</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2890,7 +2731,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>04-02-02</t>
+          <t>03-02-03</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2900,7 +2741,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>차체설계2팀</t>
+          <t>차체설계3팀</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2935,7 +2776,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04-02-03</t>
+          <t>03-02-04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2945,7 +2786,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>차체설계3팀</t>
+          <t>외장설계1팀</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2980,7 +2821,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04-02-04</t>
+          <t>03-02-05</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2990,7 +2831,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>외장설계1팀</t>
+          <t>설계팀</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -3025,7 +2866,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>04-02-05</t>
+          <t>03-02-06</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3035,7 +2876,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>설계팀</t>
+          <t>daaleiw12222222222222222222222</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -3070,7 +2911,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>04-02-06</t>
+          <t>03-02-07</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3080,7 +2921,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>daaleiw12222222222222222222222</t>
+          <t>aksdakalskdfasf</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -3115,7 +2956,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>04-02-07</t>
+          <t>03-02-08</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3125,7 +2966,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>aksdakalskdfasf</t>
+          <t>1212123124k</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3160,7 +3001,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>04-02-08</t>
+          <t>03-02-09</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3170,7 +3011,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1212123124k</t>
+          <t>외장설계2팀</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3205,22 +3046,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>04-02-09</t>
+          <t>03-03-00</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>검토중</t>
+          <t>실 추천</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>외장설계2팀</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>팀 코디</t>
+          <t>클클클</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3230,17 +3071,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>11라ㅏ아</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>리이니</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>ㄹㅇ라</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3250,12 +3091,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>04-03-00</t>
+          <t>04-00-00</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>실 추천</t>
+          <t>경영층 특강 참석자 선정</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3265,7 +3106,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>클클클</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3289,23 +3130,23 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06-00-00</t>
+          <t>04-01-00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>경영층 특강 참석자 선정</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>차체실</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3334,13 +3175,13 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06-01-00</t>
+          <t>04-02-00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3350,7 +3191,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>차체실</t>
+          <t>클로저실</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3385,7 +3226,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06-02-00</t>
+          <t>04-03-00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3395,7 +3236,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>클로저실</t>
+          <t>선행실</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3430,7 +3271,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06-03-00</t>
+          <t>04-04-00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3440,7 +3281,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>선행실</t>
+          <t>외장실</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3475,17 +3316,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06-04-00</t>
+          <t>05-00-00</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>센터 주간이슈 논의회</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>외장실</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3514,18 +3355,18 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>07-00-00</t>
+          <t>06-00-00</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>센터 주간이슈 논의회</t>
+          <t>경영층 보고</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3565,17 +3406,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>08-00-00</t>
+          <t>06-01-00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>경영층 보고</t>
+          <t>완료</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>차체설계1팀</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3604,23 +3445,23 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>08-01-00</t>
+          <t>06-02-00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>완료</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>차체설계1팀</t>
+          <t>차체설계2팀</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3655,7 +3496,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>08-02-00</t>
+          <t>06-03-00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3665,7 +3506,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>차체설계2팀</t>
+          <t>차체설계3팀</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3700,7 +3541,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>08-03-00</t>
+          <t>06-04-00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3710,7 +3551,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>차체설계3팀</t>
+          <t>외장설계1팀</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3745,7 +3586,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>08-04-00</t>
+          <t>06-05-00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3755,7 +3596,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>외장설계1팀</t>
+          <t>dkkkkkkkkkkkkkkkkk</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3631,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>08-05-00</t>
+          <t>06-06-00</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3800,7 +3641,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>dkkkkkkkkkkkkkkkkk</t>
+          <t>daaleiw12222222222222222222222</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3835,7 +3676,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>08-06-00</t>
+          <t>06-07-00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3845,7 +3686,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>daaleiw12222222222222222222222</t>
+          <t>aksdakalskdfasf</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3880,7 +3721,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>08-07-00</t>
+          <t>06-08-00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3890,7 +3731,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>aksdakalskdfasf</t>
+          <t>1212123124k</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3925,7 +3766,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>08-08-00</t>
+          <t>06-09-00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3935,7 +3776,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1212123124k</t>
+          <t>외장설계2팀</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3970,17 +3811,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>08-09-00</t>
+          <t>07-00-00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>자동화 프로그램 개발</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>외장설계2팀</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4009,7 +3850,7 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>